<commit_message>
update test case with empty cell
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/sample_data.xlsx
+++ b/src/test/resources/excel/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\n2mix\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB2298EF-1943-4453-8E29-91FBCAC4578E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF0D708-E2B7-4009-8BC3-2CE619016834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E77157C-6A11-474A-957A-4C9EFDD96AE5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Achieved</t>
+  </si>
+  <si>
+    <t>Dr</t>
+  </si>
+  <si>
+    <t>Bachelor</t>
   </si>
 </sst>
 </file>
@@ -433,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C3B371-45CC-4419-8D55-A59D75FA4FFE}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +455,7 @@
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +471,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -480,8 +492,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -499,7 +514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -515,6 +530,9 @@
       </c>
       <c r="E4" t="s">
         <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed load content with null cell
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/sample_data.xlsx
+++ b/src/test/resources/excel/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\n2mix\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF0D708-E2B7-4009-8BC3-2CE619016834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C7A6C2-E773-40A7-A0F2-FB564327451B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E77157C-6A11-474A-957A-4C9EFDD96AE5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Bachelor</t>
+  </si>
+  <si>
+    <t>Thái Minh</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C3B371-45CC-4419-8D55-A59D75FA4FFE}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,6 +544,22 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>